<commit_message>
Test cases for automationpractice.com searchFunctions tests completes
</commit_message>
<xml_diff>
--- a/com.automationpractice/src/test/resources/test_data.xlsx
+++ b/com.automationpractice/src/test/resources/test_data.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yahya\IdeaProjects\SeleniumBootcamp\com.automationpractice\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25686107-9395-48BE-8B28-D93A9C4B0D44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBF3F433-1E6A-4F1A-B553-F7CD7435CD15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14540" xr2:uid="{5DC96F64-0600-4540-8EF4-E6AE23C27A48}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14540" activeTab="1" xr2:uid="{5DC96F64-0600-4540-8EF4-E6AE23C27A48}"/>
   </bookViews>
   <sheets>
     <sheet name="Filters" sheetId="1" r:id="rId1"/>
+    <sheet name="SearchFunction" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="31">
   <si>
     <t>Assertions</t>
   </si>
@@ -119,6 +120,15 @@
   </si>
   <si>
     <t>Condition: New</t>
+  </si>
+  <si>
+    <t>"DRESSES"</t>
+  </si>
+  <si>
+    <t>PRICE DROP</t>
+  </si>
+  <si>
+    <t>10029 Not found</t>
   </si>
 </sst>
 </file>
@@ -476,8 +486,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06C7C825-8D82-4132-9F2A-6781F4BC04E3}">
   <dimension ref="A1:A28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A29" sqref="A29"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A34" sqref="A34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -630,4 +640,42 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{991C99D1-5A5D-46C1-A16E-D4743620B50F}">
+  <dimension ref="A1:A4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="14.81640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Test cases for adding items to cart on automationpractice.com added
</commit_message>
<xml_diff>
--- a/com.automationpractice/src/test/resources/test_data.xlsx
+++ b/com.automationpractice/src/test/resources/test_data.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yahya\IdeaProjects\SeleniumBootcamp\com.automationpractice\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBF3F433-1E6A-4F1A-B553-F7CD7435CD15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{617CAD36-89B5-4560-BDF2-D9F3DFBF2A64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14540" activeTab="1" xr2:uid="{5DC96F64-0600-4540-8EF4-E6AE23C27A48}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14540" activeTab="2" xr2:uid="{5DC96F64-0600-4540-8EF4-E6AE23C27A48}"/>
   </bookViews>
   <sheets>
     <sheet name="Filters" sheetId="1" r:id="rId1"/>
     <sheet name="SearchFunction" sheetId="2" r:id="rId2"/>
+    <sheet name="AddingToCart" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="32">
   <si>
     <t>Assertions</t>
   </si>
@@ -129,6 +130,9 @@
   </si>
   <si>
     <t>10029 Not found</t>
+  </si>
+  <si>
+    <t>Product successfully added to your shopping cart</t>
   </si>
 </sst>
 </file>
@@ -164,11 +168,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyProtection="1">
       <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -646,7 +653,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{991C99D1-5A5D-46C1-A16E-D4743620B50F}">
   <dimension ref="A1:A4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
@@ -678,4 +685,33 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0002D0A1-2CD6-45E4-97B6-136FF9B54B46}">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="9.453125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" ht="87" x14ac:dyDescent="0.35">
+      <c r="A2" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
added data provider and a test case
</commit_message>
<xml_diff>
--- a/com.automationpractice/src/test/resources/test_data.xlsx
+++ b/com.automationpractice/src/test/resources/test_data.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yahya\IdeaProjects\SeleniumBootcamp\com.automationpractice\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{617CAD36-89B5-4560-BDF2-D9F3DFBF2A64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8C5DD1B-1A1D-4D6D-AB18-F09E6EB3C4C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14540" activeTab="2" xr2:uid="{5DC96F64-0600-4540-8EF4-E6AE23C27A48}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14540" xr2:uid="{5DC96F64-0600-4540-8EF4-E6AE23C27A48}"/>
   </bookViews>
   <sheets>
     <sheet name="Filters" sheetId="1" r:id="rId1"/>
     <sheet name="SearchFunction" sheetId="2" r:id="rId2"/>
     <sheet name="AddingToCart" sheetId="3" r:id="rId3"/>
+    <sheet name="EmailData" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="43">
   <si>
     <t>Assertions</t>
   </si>
@@ -133,6 +134,39 @@
   </si>
   <si>
     <t>Product successfully added to your shopping cart</t>
+  </si>
+  <si>
+    <t>yahyaq91@gmail.com</t>
+  </si>
+  <si>
+    <t>fddfasdfd</t>
+  </si>
+  <si>
+    <t>yahyaq91@yahoo.com</t>
+  </si>
+  <si>
+    <t>*&amp;(^(*&amp;%%^&amp;$</t>
+  </si>
+  <si>
+    <t>yahyaq91@live.com</t>
+  </si>
+  <si>
+    <t>nufc@hotmail.com</t>
+  </si>
+  <si>
+    <t>saddf7463</t>
+  </si>
+  <si>
+    <t>realmadrid@live.com</t>
+  </si>
+  <si>
+    <t>dsda%%^</t>
+  </si>
+  <si>
+    <t>User</t>
+  </si>
+  <si>
+    <t>Password</t>
   </si>
 </sst>
 </file>
@@ -168,7 +202,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyProtection="1">
@@ -176,6 +210,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -493,8 +530,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06C7C825-8D82-4132-9F2A-6781F4BC04E3}">
   <dimension ref="A1:A28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A34" sqref="A34"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -691,7 +728,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0002D0A1-2CD6-45E4-97B6-136FF9B54B46}">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -714,4 +751,71 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B70D3569-4D22-41CD-AF0D-ECE17BE608EC}">
+  <dimension ref="A1:B6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="20.08984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.1796875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B4" s="4">
+        <v>213243314</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>37</v>
+      </c>
+      <c r="B5" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>39</v>
+      </c>
+      <c r="B6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Completed end to end test cases
</commit_message>
<xml_diff>
--- a/com.automationpractice/src/test/resources/test_data.xlsx
+++ b/com.automationpractice/src/test/resources/test_data.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yahya\IdeaProjects\SeleniumBootcamp\com.automationpractice\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8C5DD1B-1A1D-4D6D-AB18-F09E6EB3C4C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2744E7D-CE31-4AE9-98A2-F1428BC7E40A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14540" xr2:uid="{5DC96F64-0600-4540-8EF4-E6AE23C27A48}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14540" activeTab="4" xr2:uid="{5DC96F64-0600-4540-8EF4-E6AE23C27A48}"/>
   </bookViews>
   <sheets>
     <sheet name="Filters" sheetId="1" r:id="rId1"/>
     <sheet name="SearchFunction" sheetId="2" r:id="rId2"/>
     <sheet name="AddingToCart" sheetId="3" r:id="rId3"/>
     <sheet name="EmailData" sheetId="4" r:id="rId4"/>
+    <sheet name="EndToEnd" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="48">
   <si>
     <t>Assertions</t>
   </si>
@@ -167,6 +168,21 @@
   </si>
   <si>
     <t>Password</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Assertions </t>
+  </si>
+  <si>
+    <t>MY WISHLISTS</t>
+  </si>
+  <si>
+    <t>YOUR PERSONAL INFORMATION</t>
+  </si>
+  <si>
+    <t>MY ADDRESSES</t>
+  </si>
+  <si>
+    <t>CREDIT SLIPS</t>
   </si>
 </sst>
 </file>
@@ -530,7 +546,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06C7C825-8D82-4132-9F2A-6781F4BC04E3}">
   <dimension ref="A1:A28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -818,4 +834,47 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A94BA265-5162-421E-8A53-A7CFA27B884C}">
+  <dimension ref="A1:A5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="27.7265625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>47</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
I have added 3 end_to_end test cases. long way to go
</commit_message>
<xml_diff>
--- a/com.automationpractice/src/test/resources/test_data.xlsx
+++ b/com.automationpractice/src/test/resources/test_data.xlsx
@@ -8,13 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fatemazannat/IdeaProjects/SeleniumBootcamp/com.automationpractice/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12784EAE-39B9-5941-B0B6-6C93A5C823D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{531CAA3A-3242-5C4A-A3E3-AD5B35CA61BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16460" activeTab="1" xr2:uid="{AB0847C3-4333-C048-B23A-712C278E2CAB}"/>
+    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16420" activeTab="6" xr2:uid="{AB0847C3-4333-C048-B23A-712C278E2CAB}"/>
   </bookViews>
   <sheets>
     <sheet name="FilteringByColor" sheetId="1" r:id="rId1"/>
     <sheet name="AddToCartConfirmation" sheetId="2" r:id="rId2"/>
+    <sheet name="LocationConfirmation" sheetId="3" r:id="rId3"/>
+    <sheet name="Special" sheetId="5" r:id="rId4"/>
+    <sheet name="WishListConfirmation" sheetId="6" r:id="rId5"/>
+    <sheet name="AddressConfirmation" sheetId="7" r:id="rId6"/>
+    <sheet name="FilterConfirmation" sheetId="9" r:id="rId7"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -36,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="14">
   <si>
     <t>Assertions</t>
   </si>
@@ -60,13 +65,31 @@
   </si>
   <si>
     <t>Product successfully added to your shopping cart</t>
+  </si>
+  <si>
+    <t>Assersion</t>
+  </si>
+  <si>
+    <t>22204 Not found</t>
+  </si>
+  <si>
+    <t>PRICE DROP</t>
+  </si>
+  <si>
+    <t>MY WISHLISTS</t>
+  </si>
+  <si>
+    <t>MY ADDRESSES</t>
+  </si>
+  <si>
+    <t>Size: S</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -77,6 +100,19 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -102,9 +138,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -466,7 +504,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7408FC0-2178-8E47-8EDC-D6842E937231}">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
@@ -488,4 +526,135 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{762BE098-30D5-524F-A1BF-A71626EA48F7}">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="23.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41F39FC6-7276-F74E-9F2E-D6ACFAA6418C}">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3ADCD698-CAF9-FA41-949D-C2B08D8EEC53}">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="19.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48E24ACC-60CD-1C46-AD9B-3B16F65694A6}">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G20" sqref="G20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="20.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76006653-875D-904D-9C2A-086F5F5C1336}">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" s="3" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
This is the final push for this bootcamp where I have finished working on booking and marketWatch
</commit_message>
<xml_diff>
--- a/com.automationpractice/src/test/resources/test_data.xlsx
+++ b/com.automationpractice/src/test/resources/test_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fatemazannat/IdeaProjects/SeleniumBootcamp/com.automationpractice/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{531CAA3A-3242-5C4A-A3E3-AD5B35CA61BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59113418-C6CD-0C48-86EE-291397233C97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16420" activeTab="6" xr2:uid="{AB0847C3-4333-C048-B23A-712C278E2CAB}"/>
+    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16380" activeTab="7" xr2:uid="{AB0847C3-4333-C048-B23A-712C278E2CAB}"/>
   </bookViews>
   <sheets>
     <sheet name="FilteringByColor" sheetId="1" r:id="rId1"/>
@@ -20,6 +20,7 @@
     <sheet name="WishListConfirmation" sheetId="6" r:id="rId5"/>
     <sheet name="AddressConfirmation" sheetId="7" r:id="rId6"/>
     <sheet name="FilterConfirmation" sheetId="9" r:id="rId7"/>
+    <sheet name="endToEnd" sheetId="10" r:id="rId8"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -41,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="16">
   <si>
     <t>Assertions</t>
   </si>
@@ -83,6 +84,12 @@
   </si>
   <si>
     <t>Size: S</t>
+  </si>
+  <si>
+    <t>CREDIT SLIPS</t>
+  </si>
+  <si>
+    <t>Condition: New</t>
   </si>
 </sst>
 </file>
@@ -138,11 +145,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -640,7 +650,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76006653-875D-904D-9C2A-086F5F5C1336}">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
@@ -657,4 +667,47 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E73CA520-C242-854E-9A6B-D57D30C2F10E}">
+  <dimension ref="A1:A5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="19.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>